<commit_message>
Fix the issue that only one(last one processed) document in output manifest for one type i.e Audio now can have doc1.wav, doc2.wav, doc3.mp3, ..., docN.xxx
</commit_message>
<xml_diff>
--- a/testdata/metadata.xlsx
+++ b/testdata/metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -123,7 +123,7 @@
     <t>Long form description of the collection</t>
   </si>
   <si>
-    <t>Item</t>
+    <t>Item Name</t>
   </si>
   <si>
     <t>File Name</t>
@@ -219,7 +219,7 @@
     <t>RB_I_3</t>
   </si>
   <si>
-    <t>RB_I_3.wav,RB_I_3.mp3,RB_I_3.rtf,RB_I_3.txt</t>
+    <t>RB_I_3_01.mp3,RB_I_3_02.mp3,RB_I_3_03.mp3,RB_I_3.mp3,RB_I_3-raw.txt,RB_I_3.txt,RB_I_3_01.wav,RB_I_3_02.wav,RB_I_3_03.wav,RB_I_3.mkv,RB_I_3-raw.rtf,RB_I_3.rtf,RB_I_3.wav</t>
   </si>
   <si>
     <t>ID</t>
@@ -355,7 +355,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -395,9 +395,24 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Droid Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Droid Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Droid Sans"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -444,7 +459,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -485,19 +500,27 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -531,10 +554,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="10.5296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.662962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="41"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.5296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="10.5348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.6651162790698"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="40.9953488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.5348837209302"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -698,16 +721,16 @@
   </sheetPr>
   <dimension ref="A2:C13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.662962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="87.6666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.662962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6651162790698"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="87.6604651162791"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5348837209302"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -848,363 +871,355 @@
   </sheetPr>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.662962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="25.7185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.162962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.66296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.837037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2037037037037"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.0037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.5296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="41.293023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="41.293023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="10" width="41.293023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="0" t="str">
+      <c r="C2" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B2, 6,1))</f>
         <v>MQ Emotional Prosody Sentence 3</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="0" t="str">
+      <c r="F2" s="10" t="str">
         <f aca="false">VLOOKUP(MID(B2,4,1),Lists!$G$7:$H$12,2,0)</f>
         <v>afraid</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="0" t="str">
+      <c r="L2" s="10" t="str">
         <f aca="false">MID(B2,1,2)</f>
         <v>AJ</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="0" t="str">
+      <c r="C3" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B3, 6,1))</f>
         <v>MQ Emotional Prosody Sentence 6</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="0" t="str">
+      <c r="F3" s="10" t="str">
         <f aca="false">VLOOKUP(MID(B3,4,1),Lists!$G$7:$H$12,2,0)</f>
         <v>sad</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="0" t="str">
+      <c r="L3" s="10" t="str">
         <f aca="false">MID(B3,1,2)</f>
         <v>AM</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="0" t="str">
+      <c r="C4" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B4, 6,1))</f>
         <v>MQ Emotional Prosody Sentence 3</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="0" t="str">
+      <c r="F4" s="10" t="str">
         <f aca="false">VLOOKUP(MID(B4,4,1),Lists!$G$7:$H$12,2,0)</f>
         <v>afraid</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L4" s="0" t="str">
+      <c r="L4" s="10" t="str">
         <f aca="false">MID(B4,1,2)</f>
         <v>BN</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="0" t="str">
+      <c r="C5" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B5, 6,1))</f>
         <v>MQ Emotional Prosody Sentence 1</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="0" t="str">
+      <c r="F5" s="10" t="str">
         <f aca="false">VLOOKUP(MID(B5,4,1),Lists!$G$7:$H$12,2,0)</f>
         <v>tender</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="K5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="0" t="str">
+      <c r="L5" s="10" t="str">
         <f aca="false">MID(B5,1,2)</f>
         <v>CG</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="0" t="str">
+      <c r="C6" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B6, 6,1))</f>
         <v>MQ Emotional Prosody Sentence 5</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="0" t="str">
+      <c r="F6" s="10" t="str">
         <f aca="false">VLOOKUP(MID(B6,4,1),Lists!$G$7:$H$12,2,0)</f>
         <v>neutral</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="K6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L6" s="0" t="str">
+      <c r="L6" s="10" t="str">
         <f aca="false">MID(B6,1,2)</f>
         <v>ET</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="0" t="str">
+      <c r="C7" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B7, 6,1))</f>
         <v>MQ Emotional Prosody Sentence 6</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="0" t="str">
+      <c r="F7" s="10" t="str">
         <f aca="false">VLOOKUP(MID(B7,4,1),Lists!$G$7:$H$12,2,0)</f>
         <v>tender</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="K7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="0" t="str">
+      <c r="L7" s="10" t="str">
         <f aca="false">MID(B7,1,2)</f>
         <v>LD</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="0" t="str">
+      <c r="C8" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B8, 6,1))</f>
         <v>MQ Emotional Prosody Sentence 2</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="0" t="str">
+      <c r="F8" s="10" t="str">
         <f aca="false">VLOOKUP(MID(B8,4,1),Lists!$G$7:$H$12,2,0)</f>
         <v>happy</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="K8" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="0" t="str">
+      <c r="L8" s="10" t="str">
         <f aca="false">MID(B8,1,2)</f>
         <v>MC</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="0" t="str">
+      <c r="C9" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B9, 6,1))</f>
         <v>MQ Emotional Prosody Sentence 3</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="0" t="str">
+      <c r="F9" s="10" t="str">
         <f aca="false">VLOOKUP(MID(B9,4,1),Lists!$G$7:$H$12,2,0)</f>
         <v>irritated</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="K9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L9" s="0" t="str">
+      <c r="L9" s="10" t="str">
         <f aca="false">MID(B9,1,2)</f>
         <v>RB</v>
       </c>
@@ -1234,7 +1249,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,9 +1376,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.5296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8325581395349"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.5348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1373,7 +1388,7 @@
       <c r="B1" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>39</v>
       </c>
       <c r="D1" s="0" t="s">

</xml_diff>

<commit_message>
Change sheet name of files
</commit_message>
<xml_diff>
--- a/testdata/metadata.xlsx
+++ b/testdata/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Collection" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Recordings" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Files" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Speakers" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Lists" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
@@ -721,7 +721,7 @@
   </sheetPr>
   <dimension ref="A2:C13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -871,7 +871,7 @@
   </sheetPr>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -882,7 +882,7 @@
     <col collapsed="false" hidden="false" max="1025" min="3" style="10" width="41.293023255814"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
         <v>33</v>
       </c>
@@ -920,7 +920,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Deal with double quotes and spaces in doc name
</commit_message>
<xml_diff>
--- a/testdata/metadata.xlsx
+++ b/testdata/metadata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="108">
   <si>
     <t>This spreadsheet collects information about a corpus for inclusion in HCS vLab. The intention is to collect meta-data about the different files that make up the corpus so that they can be presented in the HCS vLab.</t>
   </si>
@@ -162,7 +162,7 @@
     <t>AJ_F_3</t>
   </si>
   <si>
-    <t>AJ_F_3.wav</t>
+    <t>"test space in file name", AJ_F_3.wav, ,,ingest_xlsx.py, “/tmp”, 'tmp'</t>
   </si>
   <si>
     <t>spoken</t>
@@ -180,48 +180,72 @@
     <t>individual</t>
   </si>
   <si>
+    <t>AJ</t>
+  </si>
+  <si>
     <t>AM_S_6</t>
   </si>
   <si>
     <t>AM_S_6.wav</t>
   </si>
   <si>
+    <t>AM</t>
+  </si>
+  <si>
     <t>BN_F_3</t>
   </si>
   <si>
     <t>BN_F_3.wav</t>
   </si>
   <si>
+    <t>BN</t>
+  </si>
+  <si>
     <t>CG_T_1</t>
   </si>
   <si>
     <t>CG_T_1.wav</t>
   </si>
   <si>
+    <t>CG</t>
+  </si>
+  <si>
     <t>ET_N_5</t>
   </si>
   <si>
     <t>ET_N_5.wav</t>
   </si>
   <si>
+    <t>ET</t>
+  </si>
+  <si>
     <t>LD_T_6</t>
   </si>
   <si>
     <t>LD_T_6.wav</t>
   </si>
   <si>
+    <t>LD</t>
+  </si>
+  <si>
     <t>MC_H_2</t>
   </si>
   <si>
     <t>MC_H_2.wav</t>
   </si>
   <si>
+    <t>MC</t>
+  </si>
+  <si>
     <t>RB_I_3</t>
   </si>
   <si>
     <t>RB_I_3_01.mp3,RB_I_3_02.mp3,RB_I_3_03.mp3,RB_I_3.mp3,RB_I_3-raw.txt,RB_I_3.txt,RB_I_3_01.wav,RB_I_3_02.wav,RB_I_3_03.wav,RB_I_3.mkv,RB_I_3-raw.rtf,RB_I_3.rtf,RB_I_3.wav</t>
   </si>
   <si>
+    <t>RB</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
@@ -231,43 +255,19 @@
     <t>Age</t>
   </si>
   <si>
-    <t>AJ</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
-    <t>AM</t>
-  </si>
-  <si>
-    <t>BN</t>
-  </si>
-  <si>
     <t>BS</t>
   </si>
   <si>
     <t>female</t>
   </si>
   <si>
-    <t>CG</t>
-  </si>
-  <si>
     <t>CW</t>
   </si>
   <si>
-    <t>ET</t>
-  </si>
-  <si>
-    <t>LD</t>
-  </si>
-  <si>
-    <t>MC</t>
-  </si>
-  <si>
     <t>MH</t>
-  </si>
-  <si>
-    <t>RB</t>
   </si>
   <si>
     <t>communication context</t>
@@ -872,7 +872,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -920,7 +920,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="33.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
         <v>45</v>
       </c>
@@ -929,14 +929,14 @@
       </c>
       <c r="C2" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B2, 6,1))</f>
-        <v>MQ Emotional Prosody Sentence 3</v>
+        <v>MQ Emotional Prosody Sentence  </v>
       </c>
       <c r="D2" s="10" t="s">
         <v>21</v>
       </c>
       <c r="F2" s="10" t="str">
         <f aca="false">VLOOKUP(MID(B2,4,1),Lists!$G$7:$H$12,2,0)</f>
-        <v>afraid</v>
+        <v>sad</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>47</v>
@@ -953,17 +953,16 @@
       <c r="K2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="10" t="str">
-        <f aca="false">MID(B2,1,2)</f>
-        <v>AJ</v>
+      <c r="L2" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B3, 6,1))</f>
@@ -991,17 +990,16 @@
       <c r="K3" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="10" t="str">
-        <f aca="false">MID(B3,1,2)</f>
-        <v>AM</v>
+      <c r="L3" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C4" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B4, 6,1))</f>
@@ -1029,17 +1027,16 @@
       <c r="K4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L4" s="10" t="str">
-        <f aca="false">MID(B4,1,2)</f>
-        <v>BN</v>
+      <c r="L4" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C5" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B5, 6,1))</f>
@@ -1067,17 +1064,16 @@
       <c r="K5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="10" t="str">
-        <f aca="false">MID(B5,1,2)</f>
-        <v>CG</v>
+      <c r="L5" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C6" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B6, 6,1))</f>
@@ -1105,17 +1101,16 @@
       <c r="K6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L6" s="10" t="str">
-        <f aca="false">MID(B6,1,2)</f>
-        <v>ET</v>
+      <c r="L6" s="10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C7" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B7, 6,1))</f>
@@ -1143,17 +1138,16 @@
       <c r="K7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="10" t="str">
-        <f aca="false">MID(B7,1,2)</f>
-        <v>LD</v>
+      <c r="L7" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C8" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B8, 6,1))</f>
@@ -1181,17 +1175,16 @@
       <c r="K8" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="10" t="str">
-        <f aca="false">MID(B8,1,2)</f>
-        <v>MC</v>
+      <c r="L8" s="10" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C9" s="10" t="str">
         <f aca="false">CONCATENATE("MQ Emotional Prosody Sentence ", MID(B9, 6,1))</f>
@@ -1219,9 +1212,8 @@
       <c r="K9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L9" s="10" t="str">
-        <f aca="false">MID(B9,1,2)</f>
-        <v>RB</v>
+      <c r="L9" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1254,101 +1246,101 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>